<commit_message>
Continuação Implementação + Correções
</commit_message>
<xml_diff>
--- a/ff_tabela_parser.xlsx
+++ b/ff_tabela_parser.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
   <si>
     <t>Símbolo</t>
   </si>
@@ -33,16 +33,7 @@
     <t xml:space="preserve">decl-list </t>
   </si>
   <si>
-    <t xml:space="preserve">decl-list-tail </t>
-  </si>
-  <si>
-    <t xml:space="preserve">decl </t>
-  </si>
-  <si>
     <t xml:space="preserve">ident-list </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ident-list-tail </t>
   </si>
   <si>
     <t xml:space="preserve">type </t>
@@ -185,9 +176,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>id, λ</t>
-  </si>
-  <si>
     <t>id, read, write, if, do, λ</t>
   </si>
   <si>
@@ -206,9 +194,6 @@
     <t>is</t>
   </si>
   <si>
-    <t>end, while, stop</t>
-  </si>
-  <si>
     <t>)</t>
   </si>
   <si>
@@ -231,6 +216,21 @@
   </si>
   <si>
     <t>id, if, do, read, write</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>end, while</t>
+  </si>
+  <si>
+    <t>stop, end, while</t>
+  </si>
+  <si>
+    <t>;, ), &gt;, =, &gt;=, &lt;, &lt;=, &lt;&gt;</t>
+  </si>
+  <si>
+    <t>and, *, /, or, +, -</t>
   </si>
 </sst>
 </file>
@@ -568,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -589,7 +589,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -600,51 +600,51 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
         <v>63</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -652,10 +652,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -663,10 +663,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -674,10 +674,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -685,10 +685,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -696,10 +696,10 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -710,7 +710,7 @@
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -718,10 +718,10 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -729,10 +729,10 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -740,10 +740,10 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -751,10 +751,10 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -762,10 +762,10 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -773,10 +773,10 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -784,10 +784,10 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -795,10 +795,10 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -806,10 +806,10 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -817,10 +817,10 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -828,10 +828,10 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -839,10 +839,10 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -850,10 +850,10 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -861,10 +861,10 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -872,10 +872,10 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -883,10 +883,10 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -894,10 +894,10 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -905,10 +905,10 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -916,10 +916,10 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -927,10 +927,10 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -938,43 +938,10 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Huston, we have a problem.
</commit_message>
<xml_diff>
--- a/ff_tabela_parser.xlsx
+++ b/ff_tabela_parser.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\tp_compiladores\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
   <si>
     <t>Símbolo</t>
   </si>
@@ -218,26 +223,29 @@
     <t>id, if, do, read, write</t>
   </si>
   <si>
-    <t>stop</t>
-  </si>
-  <si>
     <t>end, while</t>
   </si>
   <si>
-    <t>stop, end, while</t>
-  </si>
-  <si>
     <t>;, ), &gt;, =, &gt;=, &lt;, &lt;=, &lt;&gt;</t>
   </si>
   <si>
-    <t>and, *, /, or, +, -</t>
+    <t>stop, id, read, write, if, do</t>
+  </si>
+  <si>
+    <t>stop, id, read, write, if, do, end, while</t>
+  </si>
+  <si>
+    <t>or, +, -, ;, ), &gt;, =, &gt;=, &lt;, &lt;=, &lt;&gt;</t>
+  </si>
+  <si>
+    <t>and, *, /, or, +, -, ;, ), &gt;, =, &gt;=, &lt;, &lt;=, &lt;&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,13 +288,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -324,9 +340,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -358,9 +374,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -392,9 +409,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -567,21 +585,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +610,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -603,7 +621,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -614,7 +632,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -622,10 +640,10 @@
         <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -633,10 +651,10 @@
         <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -647,7 +665,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -658,7 +676,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -669,7 +687,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -680,7 +698,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -688,10 +706,10 @@
         <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -699,10 +717,10 @@
         <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -713,7 +731,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -724,7 +742,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -735,7 +753,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -746,7 +764,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -757,7 +775,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -768,7 +786,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -779,7 +797,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -790,7 +808,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -801,7 +819,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -812,7 +830,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -823,7 +841,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -834,7 +852,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -842,10 +860,10 @@
         <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -853,10 +871,10 @@
         <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -864,10 +882,10 @@
         <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -875,10 +893,10 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -886,10 +904,10 @@
         <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -897,10 +915,10 @@
         <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -911,7 +929,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -922,7 +940,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -933,7 +951,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -941,7 +959,7 @@
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -951,24 +969,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>